<commit_message>
added feature with election map and wrote markdown text in the main page
</commit_message>
<xml_diff>
--- a/data/interim/elections/elections_county.xlsx
+++ b/data/interim/elections/elections_county.xlsx
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>6.728391814403703</v>
+        <v>42.44305329054659</v>
       </c>
     </row>
     <row r="3">
@@ -477,7 +477,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>5.642640381499989</v>
+        <v>43.61010336094188</v>
       </c>
     </row>
     <row r="4">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>5.287057264181047</v>
+        <v>44.28217274980977</v>
       </c>
     </row>
     <row r="5">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>5.55720433298709</v>
+        <v>48.82771924617896</v>
       </c>
     </row>
     <row r="6">
@@ -522,7 +522,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>5.388888888888889</v>
+        <v>47.98148148148148</v>
       </c>
     </row>
     <row r="7">
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>6.06261607853542</v>
+        <v>31.63969222605466</v>
       </c>
     </row>
     <row r="8">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>5.293329761585856</v>
+        <v>41.21618001607286</v>
       </c>
     </row>
     <row r="9">
@@ -567,7 +567,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>5.637007437323133</v>
+        <v>41.34326872484749</v>
       </c>
     </row>
     <row r="10">
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>6.030942801443445</v>
+        <v>48.19776846820689</v>
       </c>
     </row>
     <row r="11">
@@ -597,7 +597,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>6.137954584258153</v>
+        <v>39.76011610039269</v>
       </c>
     </row>
     <row r="12">
@@ -612,7 +612,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>5.813168037509437</v>
+        <v>48.96491437199507</v>
       </c>
     </row>
     <row r="13">
@@ -627,7 +627,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>6.33646178050236</v>
+        <v>39.98806488363262</v>
       </c>
     </row>
     <row r="14">
@@ -642,7 +642,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>5.568794682051925</v>
+        <v>46.22475856014047</v>
       </c>
     </row>
     <row r="15">
@@ -657,7 +657,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>6.841130932346011</v>
+        <v>40.37571524739145</v>
       </c>
     </row>
     <row r="16">
@@ -672,7 +672,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>7.060996143609799</v>
+        <v>43.29476943131824</v>
       </c>
     </row>
     <row r="17">
@@ -687,7 +687,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>6.263554493659254</v>
+        <v>54.61496048520493</v>
       </c>
     </row>
     <row r="18">
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>5.51212870038832</v>
+        <v>48.01553280548691</v>
       </c>
     </row>
     <row r="19">
@@ -717,7 +717,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>7.077906119439666</v>
+        <v>44.26558531989842</v>
       </c>
     </row>
     <row r="20">
@@ -732,7 +732,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>6.298452324312222</v>
+        <v>41.14214547591727</v>
       </c>
     </row>
     <row r="21">
@@ -747,7 +747,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>6.875979574295971</v>
+        <v>42.91672986500834</v>
       </c>
     </row>
     <row r="22">
@@ -762,7 +762,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>5.144857251296757</v>
+        <v>36.68873613629655</v>
       </c>
     </row>
     <row r="23">
@@ -777,7 +777,7 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>6.42952891612409</v>
+        <v>45.68173113749521</v>
       </c>
     </row>
     <row r="24">
@@ -792,7 +792,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>7.344440220739557</v>
+        <v>35.3366802553448</v>
       </c>
     </row>
     <row r="25">
@@ -807,7 +807,7 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>4.475788538427365</v>
+        <v>46.7384865985488</v>
       </c>
     </row>
     <row r="26">
@@ -822,7 +822,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>5.897955999375878</v>
+        <v>41.40271493212669</v>
       </c>
     </row>
     <row r="27">
@@ -837,7 +837,7 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>4.545454545454546</v>
+        <v>44.90341591181927</v>
       </c>
     </row>
     <row r="28">
@@ -852,7 +852,7 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>5.226102037118525</v>
+        <v>31.11329692232029</v>
       </c>
     </row>
     <row r="29">
@@ -867,7 +867,7 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>6.35346655239298</v>
+        <v>39.71762370878253</v>
       </c>
     </row>
     <row r="30">
@@ -882,7 +882,7 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>8.006505511614007</v>
+        <v>28.91977925742643</v>
       </c>
     </row>
     <row r="31">
@@ -897,7 +897,7 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>4.24068399511432</v>
+        <v>33.89118649152506</v>
       </c>
     </row>
     <row r="32">
@@ -912,7 +912,7 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>6.222837583169878</v>
+        <v>45.40979193107957</v>
       </c>
     </row>
     <row r="33">
@@ -927,7 +927,7 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>4.711767067033069</v>
+        <v>42.88140303208078</v>
       </c>
     </row>
     <row r="34">
@@ -942,7 +942,7 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>8.219581294381692</v>
+        <v>32.86728724382795</v>
       </c>
     </row>
     <row r="35">
@@ -957,7 +957,7 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>6.704353862937618</v>
+        <v>39.85916889814539</v>
       </c>
     </row>
     <row r="36">
@@ -972,7 +972,7 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>6.198528604370265</v>
+        <v>49.97803887119797</v>
       </c>
     </row>
     <row r="37">
@@ -987,7 +987,7 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>6.185498368732938</v>
+        <v>47.75950462747187</v>
       </c>
     </row>
     <row r="38">
@@ -1002,7 +1002,7 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>5.824115895012095</v>
+        <v>37.65609050102778</v>
       </c>
     </row>
     <row r="39">
@@ -1017,7 +1017,7 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>4.9138558602281</v>
+        <v>47.62193642319825</v>
       </c>
     </row>
     <row r="40">
@@ -1032,7 +1032,7 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>5.627125631248068</v>
+        <v>40.85849737194683</v>
       </c>
     </row>
     <row r="41">
@@ -1047,7 +1047,7 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>7.311611241742246</v>
+        <v>40.13828238719069</v>
       </c>
     </row>
     <row r="42">
@@ -1062,7 +1062,7 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>4.531485387164809</v>
+        <v>55.69147333534197</v>
       </c>
     </row>
     <row r="43">
@@ -1077,7 +1077,7 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>5.719470787963939</v>
+        <v>49.81266830581899</v>
       </c>
     </row>
     <row r="44">
@@ -1092,7 +1092,7 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>6.140845070422536</v>
+        <v>42.32237871674491</v>
       </c>
     </row>
     <row r="45">
@@ -1107,7 +1107,7 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>7.253623004492271</v>
+        <v>40.5015101139565</v>
       </c>
     </row>
     <row r="46">
@@ -1122,7 +1122,7 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>7.393317536575291</v>
+        <v>39.892611030195</v>
       </c>
     </row>
     <row r="47">
@@ -1137,7 +1137,7 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>7.757487216946676</v>
+        <v>48.57560262965669</v>
       </c>
     </row>
     <row r="48">
@@ -1152,7 +1152,7 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>6.619313888469095</v>
+        <v>39.94257216261146</v>
       </c>
     </row>
     <row r="49">
@@ -1167,7 +1167,7 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>5.246315542246491</v>
+        <v>51.12442017497505</v>
       </c>
     </row>
     <row r="50">
@@ -1182,7 +1182,7 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>5.722402597402597</v>
+        <v>41.88649891774892</v>
       </c>
     </row>
     <row r="51">
@@ -1197,7 +1197,7 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>7.461009094996022</v>
+        <v>31.93507855817224</v>
       </c>
     </row>
     <row r="52">
@@ -1212,7 +1212,7 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>6.316812439261418</v>
+        <v>34.31282287351031</v>
       </c>
     </row>
     <row r="53">
@@ -1227,7 +1227,7 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>7.673247542162896</v>
+        <v>31.55223403405004</v>
       </c>
     </row>
     <row r="54">
@@ -1242,7 +1242,7 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>5.866715002114676</v>
+        <v>34.36851751153002</v>
       </c>
     </row>
     <row r="55">
@@ -1257,7 +1257,7 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>5.352044225745702</v>
+        <v>60.88734989773808</v>
       </c>
     </row>
     <row r="56">
@@ -1272,7 +1272,7 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>6.796370615948351</v>
+        <v>64.99738265573198</v>
       </c>
     </row>
     <row r="57">
@@ -1287,7 +1287,7 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>6.034281132012429</v>
+        <v>61.19148651809282</v>
       </c>
     </row>
     <row r="58">
@@ -1302,7 +1302,7 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>4.575189155107187</v>
+        <v>62.37783732660782</v>
       </c>
     </row>
     <row r="59">
@@ -1317,7 +1317,7 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>5.333998005982054</v>
+        <v>77.18662195232484</v>
       </c>
     </row>
     <row r="60">
@@ -1332,7 +1332,7 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>6.022898796156537</v>
+        <v>61.28925376431174</v>
       </c>
     </row>
     <row r="61">
@@ -1347,7 +1347,7 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>4.966102498459205</v>
+        <v>62.46385056653866</v>
       </c>
     </row>
     <row r="62">
@@ -1362,7 +1362,7 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>9.079242861726017</v>
+        <v>61.80745786135584</v>
       </c>
     </row>
     <row r="63">
@@ -1377,7 +1377,7 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>7.209731428961935</v>
+        <v>57.99630971092735</v>
       </c>
     </row>
     <row r="64">
@@ -1392,7 +1392,7 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>7.716566866267464</v>
+        <v>60.12375249500999</v>
       </c>
     </row>
     <row r="65">
@@ -1407,7 +1407,7 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>6.007435247977775</v>
+        <v>68.02230574393333</v>
       </c>
     </row>
     <row r="66">
@@ -1422,7 +1422,7 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>5.966634738186462</v>
+        <v>62.51995530012772</v>
       </c>
     </row>
     <row r="67">
@@ -1437,7 +1437,7 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>6.636818540953385</v>
+        <v>59.40874374506188</v>
       </c>
     </row>
     <row r="68">
@@ -1452,7 +1452,7 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>7.862924986508364</v>
+        <v>53.91437308868502</v>
       </c>
     </row>
     <row r="69">
@@ -1467,7 +1467,7 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>5.552607640994542</v>
+        <v>64.28896300788357</v>
       </c>
     </row>
     <row r="70">
@@ -1482,7 +1482,7 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>5.133641250851821</v>
+        <v>60.53986522298781</v>
       </c>
     </row>
     <row r="71">
@@ -1497,7 +1497,7 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>6.569691188744485</v>
+        <v>56.20305234291165</v>
       </c>
     </row>
     <row r="72">
@@ -1512,7 +1512,7 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>5.550057960360768</v>
+        <v>63.2531312731488</v>
       </c>
     </row>
     <row r="73">
@@ -1527,7 +1527,7 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>5.410639714337591</v>
+        <v>52.84149367548267</v>
       </c>
     </row>
     <row r="74">
@@ -1542,7 +1542,7 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>5.264642082429502</v>
+        <v>66.96529284164859</v>
       </c>
     </row>
     <row r="75">
@@ -1557,7 +1557,7 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>6.690425453743846</v>
+        <v>48.12991402748181</v>
       </c>
     </row>
     <row r="76">
@@ -1572,7 +1572,7 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>6.303745291734773</v>
+        <v>46.16231966455831</v>
       </c>
     </row>
     <row r="77">
@@ -1587,7 +1587,7 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>7.793348550954954</v>
+        <v>42.52015371724119</v>
       </c>
     </row>
     <row r="78">
@@ -1602,7 +1602,7 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>6.011500261369576</v>
+        <v>49.1130859034675</v>
       </c>
     </row>
     <row r="79">
@@ -1617,7 +1617,7 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>7.937288858276756</v>
+        <v>34.72727869067532</v>
       </c>
     </row>
     <row r="80">
@@ -1632,7 +1632,7 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>5.227882037533512</v>
+        <v>31.66666666666666</v>
       </c>
     </row>
     <row r="81">
@@ -1647,7 +1647,7 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>7.091630273648784</v>
+        <v>34.39641011258464</v>
       </c>
     </row>
     <row r="82">
@@ -1662,7 +1662,7 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>7.479382705968808</v>
+        <v>37.49489670939822</v>
       </c>
     </row>
     <row r="83">
@@ -1677,7 +1677,7 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>7.154088050314465</v>
+        <v>32.28511530398323</v>
       </c>
     </row>
     <row r="84">
@@ -1692,7 +1692,7 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>5.827145214521452</v>
+        <v>39.22751650165016</v>
       </c>
     </row>
     <row r="85">
@@ -1707,7 +1707,7 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>7.67667972718038</v>
+        <v>40.26991728341315</v>
       </c>
     </row>
     <row r="86">
@@ -1722,7 +1722,7 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>7.570817631367236</v>
+        <v>35.17381547190583</v>
       </c>
     </row>
     <row r="87">
@@ -1737,7 +1737,7 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>7.654230451920433</v>
+        <v>33.40055611574541</v>
       </c>
     </row>
     <row r="88">
@@ -1752,7 +1752,7 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>7.5112637449195</v>
+        <v>39.83112259365449</v>
       </c>
     </row>
     <row r="89">
@@ -1767,7 +1767,7 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>8.472715201348279</v>
+        <v>35.31830137126222</v>
       </c>
     </row>
     <row r="90">
@@ -1782,7 +1782,7 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>6.495238095238095</v>
+        <v>48.17142857142857</v>
       </c>
     </row>
     <row r="91">
@@ -1797,7 +1797,7 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>7.490781387181738</v>
+        <v>32.57418788410887</v>
       </c>
     </row>
     <row r="92">
@@ -1812,7 +1812,7 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>6.387912860154603</v>
+        <v>26.68446943078004</v>
       </c>
     </row>
     <row r="93">
@@ -1827,7 +1827,7 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>10.00017876615599</v>
+        <v>59.73113570138901</v>
       </c>
     </row>
     <row r="94">
@@ -1842,7 +1842,7 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>5.257368107439153</v>
+        <v>52.26199752486593</v>
       </c>
     </row>
     <row r="95">
@@ -1857,7 +1857,7 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>6.61512027491409</v>
+        <v>50.15136638847979</v>
       </c>
     </row>
     <row r="96">
@@ -1872,7 +1872,7 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>4.879472101270369</v>
+        <v>57.62445571665844</v>
       </c>
     </row>
     <row r="97">
@@ -1887,7 +1887,7 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>5.594592428330973</v>
+        <v>56.10889951641775</v>
       </c>
     </row>
     <row r="98">
@@ -1902,7 +1902,7 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>7.739169085157006</v>
+        <v>44.58650351661569</v>
       </c>
     </row>
     <row r="99">
@@ -1917,7 +1917,7 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>4.644622016612344</v>
+        <v>64.38860267059195</v>
       </c>
     </row>
     <row r="100">
@@ -1932,7 +1932,7 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>6.706823407493766</v>
+        <v>39.13015317853558</v>
       </c>
     </row>
     <row r="101">
@@ -1947,7 +1947,7 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>5.412538573980835</v>
+        <v>62.33149261003735</v>
       </c>
     </row>
     <row r="102">
@@ -1962,7 +1962,7 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>6.508767098136419</v>
+        <v>64.74341320113834</v>
       </c>
     </row>
     <row r="103">
@@ -1977,7 +1977,7 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>4.961851871074894</v>
+        <v>55.95058909015415</v>
       </c>
     </row>
     <row r="104">
@@ -1992,7 +1992,7 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>5.813505813505813</v>
+        <v>55.62293062293062</v>
       </c>
     </row>
     <row r="105">
@@ -2007,7 +2007,7 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>6.385839121667041</v>
+        <v>58.00134438718351</v>
       </c>
     </row>
     <row r="106">
@@ -2022,7 +2022,7 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>6.190330642406372</v>
+        <v>54.45441306028516</v>
       </c>
     </row>
     <row r="107">
@@ -2037,7 +2037,7 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>6.555044867585905</v>
+        <v>65.43007222586999</v>
       </c>
     </row>
     <row r="108">
@@ -2052,7 +2052,7 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>6.460170646017064</v>
+        <v>52.01835520183552</v>
       </c>
     </row>
     <row r="109">
@@ -2067,7 +2067,7 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>5.329690044437084</v>
+        <v>55.18754657613646</v>
       </c>
     </row>
     <row r="110">
@@ -2082,7 +2082,7 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>6.90822010515904</v>
+        <v>54.0996407933781</v>
       </c>
     </row>
     <row r="111">
@@ -2097,7 +2097,7 @@
         </is>
       </c>
       <c r="C111" t="n">
-        <v>6.23931082536264</v>
+        <v>47.58662190409831</v>
       </c>
     </row>
     <row r="112">
@@ -2112,7 +2112,7 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>5.774097351756585</v>
+        <v>40.80837362924592</v>
       </c>
     </row>
     <row r="113">
@@ -2127,7 +2127,7 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>6.788179320511961</v>
+        <v>53.62192588621591</v>
       </c>
     </row>
     <row r="114">
@@ -2142,7 +2142,7 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>6.52758230537848</v>
+        <v>30.8182244667053</v>
       </c>
     </row>
     <row r="115">
@@ -2157,7 +2157,7 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>6.383096716947649</v>
+        <v>43.84982253771074</v>
       </c>
     </row>
     <row r="116">
@@ -2172,7 +2172,7 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>6.894995898277275</v>
+        <v>40.64397046759639</v>
       </c>
     </row>
     <row r="117">
@@ -2187,7 +2187,7 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>6.618790683384858</v>
+        <v>65.0799746538912</v>
       </c>
     </row>
     <row r="118">
@@ -2202,7 +2202,7 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>8.438996900535361</v>
+        <v>63.62355593124824</v>
       </c>
     </row>
     <row r="119">
@@ -2217,7 +2217,7 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>7.154660427676249</v>
+        <v>44.38736277220595</v>
       </c>
     </row>
     <row r="120">
@@ -2232,7 +2232,7 @@
         </is>
       </c>
       <c r="C120" t="n">
-        <v>6.55513552642162</v>
+        <v>70.18820879916352</v>
       </c>
     </row>
     <row r="121">
@@ -2247,7 +2247,7 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>6.137028924689361</v>
+        <v>61.91684919448937</v>
       </c>
     </row>
     <row r="122">
@@ -2262,7 +2262,7 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>7.80972994524859</v>
+        <v>50.85473432393754</v>
       </c>
     </row>
     <row r="123">
@@ -2277,7 +2277,7 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>6.855826959453902</v>
+        <v>71.81676124681306</v>
       </c>
     </row>
     <row r="124">
@@ -2292,7 +2292,7 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>5.693530079455165</v>
+        <v>61.59364358683315</v>
       </c>
     </row>
     <row r="125">
@@ -2307,7 +2307,7 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>8.023116908274948</v>
+        <v>62.3300939527976</v>
       </c>
     </row>
     <row r="126">
@@ -2322,7 +2322,7 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>6.526520236497101</v>
+        <v>71.84408709643635</v>
       </c>
     </row>
     <row r="127">
@@ -2337,7 +2337,7 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>7.731067345136046</v>
+        <v>66.68574343406696</v>
       </c>
     </row>
     <row r="128">
@@ -2352,7 +2352,7 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>6.824448529411764</v>
+        <v>51.10647624434389</v>
       </c>
     </row>
     <row r="129">
@@ -2367,7 +2367,7 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>6.25435046018201</v>
+        <v>48.31911108819511</v>
       </c>
     </row>
     <row r="130">
@@ -2382,7 +2382,7 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>5.628547403825941</v>
+        <v>62.55518183729241</v>
       </c>
     </row>
     <row r="131">
@@ -2397,7 +2397,7 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>7.657819225251076</v>
+        <v>62.83306005328961</v>
       </c>
     </row>
     <row r="132">
@@ -2412,7 +2412,7 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>6.458158333969695</v>
+        <v>67.51611812320682</v>
       </c>
     </row>
     <row r="133">
@@ -2427,7 +2427,7 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>7.724235377233522</v>
+        <v>56.03014335756969</v>
       </c>
     </row>
     <row r="134">
@@ -2442,7 +2442,7 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>6.72877170518834</v>
+        <v>54.0326900714687</v>
       </c>
     </row>
     <row r="135">
@@ -2457,7 +2457,7 @@
         </is>
       </c>
       <c r="C135" t="n">
-        <v>8.261928099408733</v>
+        <v>48.41116767319063</v>
       </c>
     </row>
     <row r="136">
@@ -2472,7 +2472,7 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>8.314332001496863</v>
+        <v>33.22385777009202</v>
       </c>
     </row>
     <row r="137">
@@ -2487,7 +2487,7 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>7.014475857378801</v>
+        <v>52.41669095501798</v>
       </c>
     </row>
     <row r="138">
@@ -2502,7 +2502,7 @@
         </is>
       </c>
       <c r="C138" t="n">
-        <v>7.101816960787971</v>
+        <v>44.74872215796739</v>
       </c>
     </row>
     <row r="139">
@@ -2517,7 +2517,7 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>4.370651486401012</v>
+        <v>65.40796963946869</v>
       </c>
     </row>
     <row r="140">
@@ -2532,7 +2532,7 @@
         </is>
       </c>
       <c r="C140" t="n">
-        <v>5.115019625378844</v>
+        <v>54.24305659064937</v>
       </c>
     </row>
     <row r="141">
@@ -2547,7 +2547,7 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>5.605697094329563</v>
+        <v>67.18839255112533</v>
       </c>
     </row>
     <row r="142">
@@ -2562,7 +2562,7 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>5.03926051088361</v>
+        <v>55.65550144120864</v>
       </c>
     </row>
     <row r="143">
@@ -2577,7 +2577,7 @@
         </is>
       </c>
       <c r="C143" t="n">
-        <v>6.48813195121466</v>
+        <v>37.93000537195837</v>
       </c>
     </row>
     <row r="144">
@@ -2592,7 +2592,7 @@
         </is>
       </c>
       <c r="C144" t="n">
-        <v>6.521420648374877</v>
+        <v>50.56193884598481</v>
       </c>
     </row>
     <row r="145">
@@ -2607,7 +2607,7 @@
         </is>
       </c>
       <c r="C145" t="n">
-        <v>5.124175861715575</v>
+        <v>61.26123048543026</v>
       </c>
     </row>
     <row r="146">
@@ -2622,7 +2622,7 @@
         </is>
       </c>
       <c r="C146" t="n">
-        <v>5.626168517965718</v>
+        <v>37.63766909142328</v>
       </c>
     </row>
     <row r="147">
@@ -2637,7 +2637,7 @@
         </is>
       </c>
       <c r="C147" t="n">
-        <v>6.722341086341363</v>
+        <v>62.33694526882463</v>
       </c>
     </row>
     <row r="148">
@@ -2652,7 +2652,7 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>7.051552184295547</v>
+        <v>66.55429133305239</v>
       </c>
     </row>
     <row r="149">
@@ -2667,7 +2667,7 @@
         </is>
       </c>
       <c r="C149" t="n">
-        <v>5.757333865495909</v>
+        <v>62.51247256036719</v>
       </c>
     </row>
     <row r="150">
@@ -2682,7 +2682,7 @@
         </is>
       </c>
       <c r="C150" t="n">
-        <v>7.232736836676809</v>
+        <v>50.21401681192306</v>
       </c>
     </row>
     <row r="151">
@@ -2697,7 +2697,7 @@
         </is>
       </c>
       <c r="C151" t="n">
-        <v>6.091006807595844</v>
+        <v>56.50304550340379</v>
       </c>
     </row>
     <row r="152">
@@ -2712,7 +2712,7 @@
         </is>
       </c>
       <c r="C152" t="n">
-        <v>5.946017116524029</v>
+        <v>45.14022383146808</v>
       </c>
     </row>
     <row r="153">
@@ -2727,7 +2727,7 @@
         </is>
       </c>
       <c r="C153" t="n">
-        <v>6.180652806204891</v>
+        <v>66.61908865668427</v>
       </c>
     </row>
     <row r="154">
@@ -2742,7 +2742,7 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>5.21418065019662</v>
+        <v>63.25758712814817</v>
       </c>
     </row>
     <row r="155">
@@ -2757,7 +2757,7 @@
         </is>
       </c>
       <c r="C155" t="n">
-        <v>6.948536042806469</v>
+        <v>47.16677688931642</v>
       </c>
     </row>
     <row r="156">
@@ -2772,7 +2772,7 @@
         </is>
       </c>
       <c r="C156" t="n">
-        <v>6.237675560384724</v>
+        <v>35.17244154694354</v>
       </c>
     </row>
     <row r="157">
@@ -2787,7 +2787,7 @@
         </is>
       </c>
       <c r="C157" t="n">
-        <v>4.958454507685916</v>
+        <v>56.79268799335272</v>
       </c>
     </row>
     <row r="158">
@@ -2802,7 +2802,7 @@
         </is>
       </c>
       <c r="C158" t="n">
-        <v>4.910627684633504</v>
+        <v>56.12858528474436</v>
       </c>
     </row>
     <row r="159">
@@ -2817,7 +2817,7 @@
         </is>
       </c>
       <c r="C159" t="n">
-        <v>6.399594429882752</v>
+        <v>35.79479877897507</v>
       </c>
     </row>
     <row r="160">
@@ -2832,7 +2832,7 @@
         </is>
       </c>
       <c r="C160" t="n">
-        <v>5.018486788709533</v>
+        <v>59.73487239606817</v>
       </c>
     </row>
     <row r="161">
@@ -2847,7 +2847,7 @@
         </is>
       </c>
       <c r="C161" t="n">
-        <v>5.311577010603787</v>
+        <v>70.35781726625672</v>
       </c>
     </row>
     <row r="162">
@@ -2862,7 +2862,7 @@
         </is>
       </c>
       <c r="C162" t="n">
-        <v>5.31611604896864</v>
+        <v>56.44390407512997</v>
       </c>
     </row>
     <row r="163">
@@ -2877,7 +2877,7 @@
         </is>
       </c>
       <c r="C163" t="n">
-        <v>5.870877712593268</v>
+        <v>66.02209944751381</v>
       </c>
     </row>
     <row r="164">
@@ -2892,7 +2892,7 @@
         </is>
       </c>
       <c r="C164" t="n">
-        <v>6.723336500680552</v>
+        <v>69.30070109658698</v>
       </c>
     </row>
     <row r="165">
@@ -2907,7 +2907,7 @@
         </is>
       </c>
       <c r="C165" t="n">
-        <v>4.3733681462141</v>
+        <v>58.33644162625886</v>
       </c>
     </row>
     <row r="166">
@@ -2922,7 +2922,7 @@
         </is>
       </c>
       <c r="C166" t="n">
-        <v>5.883960061596542</v>
+        <v>50.54890467438279</v>
       </c>
     </row>
     <row r="167">
@@ -2937,7 +2937,7 @@
         </is>
       </c>
       <c r="C167" t="n">
-        <v>5.702178276708052</v>
+        <v>63.20719649096721</v>
       </c>
     </row>
     <row r="168">
@@ -2952,7 +2952,7 @@
         </is>
       </c>
       <c r="C168" t="n">
-        <v>5.495757161569566</v>
+        <v>67.1735292442622</v>
       </c>
     </row>
     <row r="169">
@@ -2967,7 +2967,7 @@
         </is>
       </c>
       <c r="C169" t="n">
-        <v>6.635308090200184</v>
+        <v>38.59136441062024</v>
       </c>
     </row>
     <row r="170">
@@ -2982,7 +2982,7 @@
         </is>
       </c>
       <c r="C170" t="n">
-        <v>6.277610602471349</v>
+        <v>62.92976502977143</v>
       </c>
     </row>
     <row r="171">
@@ -2997,7 +2997,7 @@
         </is>
       </c>
       <c r="C171" t="n">
-        <v>7.706860740335228</v>
+        <v>48.65796126040543</v>
       </c>
     </row>
     <row r="172">
@@ -3012,7 +3012,7 @@
         </is>
       </c>
       <c r="C172" t="n">
-        <v>7.25729626742877</v>
+        <v>58.59530614012297</v>
       </c>
     </row>
     <row r="173">
@@ -3027,7 +3027,7 @@
         </is>
       </c>
       <c r="C173" t="n">
-        <v>5.629471570227188</v>
+        <v>64.25254173465545</v>
       </c>
     </row>
     <row r="174">
@@ -3042,7 +3042,7 @@
         </is>
       </c>
       <c r="C174" t="n">
-        <v>3.866528648846131</v>
+        <v>57.29769226085368</v>
       </c>
     </row>
     <row r="175">
@@ -3057,7 +3057,7 @@
         </is>
       </c>
       <c r="C175" t="n">
-        <v>6.282271944922548</v>
+        <v>46.97962356337793</v>
       </c>
     </row>
     <row r="176">
@@ -3072,7 +3072,7 @@
         </is>
       </c>
       <c r="C176" t="n">
-        <v>7.443703085904921</v>
+        <v>50.40450375312761</v>
       </c>
     </row>
     <row r="177">
@@ -3087,7 +3087,7 @@
         </is>
       </c>
       <c r="C177" t="n">
-        <v>5.06567559311679</v>
+        <v>40.64589485116926</v>
       </c>
     </row>
     <row r="178">
@@ -3102,7 +3102,7 @@
         </is>
       </c>
       <c r="C178" t="n">
-        <v>6.158866017311826</v>
+        <v>47.7469452566759</v>
       </c>
     </row>
     <row r="179">
@@ -3117,7 +3117,7 @@
         </is>
       </c>
       <c r="C179" t="n">
-        <v>7.694902062524323</v>
+        <v>49.54209365676482</v>
       </c>
     </row>
     <row r="180">
@@ -3132,7 +3132,7 @@
         </is>
       </c>
       <c r="C180" t="n">
-        <v>6.373965674394815</v>
+        <v>28.25562561652036</v>
       </c>
     </row>
     <row r="181">
@@ -3147,7 +3147,7 @@
         </is>
       </c>
       <c r="C181" t="n">
-        <v>13.29479768786127</v>
+        <v>21.96531791907514</v>
       </c>
     </row>
     <row r="182">
@@ -3162,7 +3162,7 @@
         </is>
       </c>
       <c r="C182" t="n">
-        <v>11.38512255736474</v>
+        <v>24.8895026745285</v>
       </c>
     </row>
     <row r="183">
@@ -3177,7 +3177,7 @@
         </is>
       </c>
       <c r="C183" t="n">
-        <v>6.438310265728499</v>
+        <v>44.27433696744762</v>
       </c>
     </row>
     <row r="184">
@@ -3192,7 +3192,7 @@
         </is>
       </c>
       <c r="C184" t="n">
-        <v>4.87699611566681</v>
+        <v>54.03539059128183</v>
       </c>
     </row>
     <row r="185">
@@ -3207,7 +3207,7 @@
         </is>
       </c>
       <c r="C185" t="n">
-        <v>6.177284574253701</v>
+        <v>33.16763844479673</v>
       </c>
     </row>
     <row r="186">
@@ -3222,7 +3222,7 @@
         </is>
       </c>
       <c r="C186" t="n">
-        <v>6.314064702968411</v>
+        <v>40.54033456540792</v>
       </c>
     </row>
     <row r="187">
@@ -3237,7 +3237,7 @@
         </is>
       </c>
       <c r="C187" t="n">
-        <v>5.947019867549669</v>
+        <v>28.99779249448124</v>
       </c>
     </row>
     <row r="188">
@@ -3252,7 +3252,7 @@
         </is>
       </c>
       <c r="C188" t="n">
-        <v>5.589960886571056</v>
+        <v>44.22533681008257</v>
       </c>
     </row>
     <row r="189">
@@ -3267,7 +3267,7 @@
         </is>
       </c>
       <c r="C189" t="n">
-        <v>5.088221104142256</v>
+        <v>48.13047074229788</v>
       </c>
     </row>
     <row r="190">
@@ -3282,7 +3282,7 @@
         </is>
       </c>
       <c r="C190" t="n">
-        <v>5.639396346306593</v>
+        <v>41.8109610802224</v>
       </c>
     </row>
     <row r="191">
@@ -3297,7 +3297,7 @@
         </is>
       </c>
       <c r="C191" t="n">
-        <v>5.375799404799595</v>
+        <v>29.44975622111062</v>
       </c>
     </row>
     <row r="192">
@@ -3312,7 +3312,7 @@
         </is>
       </c>
       <c r="C192" t="n">
-        <v>5.470469767224017</v>
+        <v>45.12200833684605</v>
       </c>
     </row>
     <row r="193">
@@ -3327,7 +3327,7 @@
         </is>
       </c>
       <c r="C193" t="n">
-        <v>5.276872964169381</v>
+        <v>32.57328990228013</v>
       </c>
     </row>
     <row r="194">
@@ -3342,7 +3342,7 @@
         </is>
       </c>
       <c r="C194" t="n">
-        <v>5.992924165512998</v>
+        <v>26.24980772188894</v>
       </c>
     </row>
     <row r="195">
@@ -3357,7 +3357,7 @@
         </is>
       </c>
       <c r="C195" t="n">
-        <v>7.702060221870048</v>
+        <v>49.85736925515055</v>
       </c>
     </row>
     <row r="196">
@@ -3372,7 +3372,7 @@
         </is>
       </c>
       <c r="C196" t="n">
-        <v>6.575437380911138</v>
+        <v>75.77342802702235</v>
       </c>
     </row>
     <row r="197">
@@ -3387,7 +3387,7 @@
         </is>
       </c>
       <c r="C197" t="n">
-        <v>7.145687073105023</v>
+        <v>65.41734679323625</v>
       </c>
     </row>
     <row r="198">
@@ -3402,7 +3402,7 @@
         </is>
       </c>
       <c r="C198" t="n">
-        <v>6.119424828948813</v>
+        <v>65.62877318795508</v>
       </c>
     </row>
     <row r="199">
@@ -3417,7 +3417,7 @@
         </is>
       </c>
       <c r="C199" t="n">
-        <v>7.233639805300163</v>
+        <v>68.74758556748823</v>
       </c>
     </row>
     <row r="200">
@@ -3432,7 +3432,7 @@
         </is>
       </c>
       <c r="C200" t="n">
-        <v>9.807297772567409</v>
+        <v>72.21570926143025</v>
       </c>
     </row>
     <row r="201">
@@ -3447,7 +3447,7 @@
         </is>
       </c>
       <c r="C201" t="n">
-        <v>7.050672462980573</v>
+        <v>65.95959399926252</v>
       </c>
     </row>
     <row r="202">
@@ -3462,7 +3462,7 @@
         </is>
       </c>
       <c r="C202" t="n">
-        <v>7.953645948769908</v>
+        <v>74.15698318715765</v>
       </c>
     </row>
     <row r="203">
@@ -3477,7 +3477,7 @@
         </is>
       </c>
       <c r="C203" t="n">
-        <v>6.915879973027647</v>
+        <v>64.0930546190155</v>
       </c>
     </row>
     <row r="204">
@@ -3492,7 +3492,7 @@
         </is>
       </c>
       <c r="C204" t="n">
-        <v>8.527939420120449</v>
+        <v>68.91215409244531</v>
       </c>
     </row>
     <row r="205">
@@ -3507,7 +3507,7 @@
         </is>
       </c>
       <c r="C205" t="n">
-        <v>6.451766422894491</v>
+        <v>62.59657026825515</v>
       </c>
     </row>
     <row r="206">
@@ -3522,7 +3522,7 @@
         </is>
       </c>
       <c r="C206" t="n">
-        <v>8.371798033895917</v>
+        <v>70.4168281596843</v>
       </c>
     </row>
     <row r="207">
@@ -3537,7 +3537,7 @@
         </is>
       </c>
       <c r="C207" t="n">
-        <v>7.176602924634421</v>
+        <v>65.56323316728266</v>
       </c>
     </row>
     <row r="208">
@@ -3552,7 +3552,7 @@
         </is>
       </c>
       <c r="C208" t="n">
-        <v>6.0744888436413</v>
+        <v>69.40980175900003</v>
       </c>
     </row>
     <row r="209">
@@ -3567,7 +3567,7 @@
         </is>
       </c>
       <c r="C209" t="n">
-        <v>7.265174635469651</v>
+        <v>72.02441505595118</v>
       </c>
     </row>
     <row r="210">
@@ -3582,7 +3582,7 @@
         </is>
       </c>
       <c r="C210" t="n">
-        <v>8.561548261845537</v>
+        <v>67.59206455135595</v>
       </c>
     </row>
     <row r="211">
@@ -3597,7 +3597,7 @@
         </is>
       </c>
       <c r="C211" t="n">
-        <v>5.859288847501654</v>
+        <v>59.40157325948979</v>
       </c>
     </row>
     <row r="212">
@@ -3612,7 +3612,7 @@
         </is>
       </c>
       <c r="C212" t="n">
-        <v>8.580299785867238</v>
+        <v>61.11991434689508</v>
       </c>
     </row>
     <row r="213">
@@ -3627,7 +3627,7 @@
         </is>
       </c>
       <c r="C213" t="n">
-        <v>8.848314606741573</v>
+        <v>69.98343416882743</v>
       </c>
     </row>
     <row r="214">
@@ -3642,7 +3642,7 @@
         </is>
       </c>
       <c r="C214" t="n">
-        <v>6.405435432868986</v>
+        <v>63.88770190582002</v>
       </c>
     </row>
     <row r="215">
@@ -3657,7 +3657,7 @@
         </is>
       </c>
       <c r="C215" t="n">
-        <v>6.145134228187919</v>
+        <v>53.85206935123043</v>
       </c>
     </row>
     <row r="216">
@@ -3672,7 +3672,7 @@
         </is>
       </c>
       <c r="C216" t="n">
-        <v>7.800465699444743</v>
+        <v>47.94465341214401</v>
       </c>
     </row>
     <row r="217">
@@ -3687,7 +3687,7 @@
         </is>
       </c>
       <c r="C217" t="n">
-        <v>8.373681642457681</v>
+        <v>47.44961153023308</v>
       </c>
     </row>
     <row r="218">
@@ -3702,7 +3702,7 @@
         </is>
       </c>
       <c r="C218" t="n">
-        <v>9.903396318123821</v>
+        <v>42.9612977702169</v>
       </c>
     </row>
     <row r="219">
@@ -3717,7 +3717,7 @@
         </is>
       </c>
       <c r="C219" t="n">
-        <v>8.020177711958535</v>
+        <v>45.10366530914477</v>
       </c>
     </row>
     <row r="220">
@@ -3732,7 +3732,7 @@
         </is>
       </c>
       <c r="C220" t="n">
-        <v>5.835196827138096</v>
+        <v>55.02299481034556</v>
       </c>
     </row>
     <row r="221">
@@ -3747,7 +3747,7 @@
         </is>
       </c>
       <c r="C221" t="n">
-        <v>7.584698195216028</v>
+        <v>53.24256642008002</v>
       </c>
     </row>
     <row r="222">
@@ -3762,7 +3762,7 @@
         </is>
       </c>
       <c r="C222" t="n">
-        <v>4.49824091137544</v>
+        <v>50.94236890601442</v>
       </c>
     </row>
     <row r="223">
@@ -3777,7 +3777,7 @@
         </is>
       </c>
       <c r="C223" t="n">
-        <v>7.428325533860471</v>
+        <v>61.16400408799957</v>
       </c>
     </row>
     <row r="224">
@@ -3792,7 +3792,7 @@
         </is>
       </c>
       <c r="C224" t="n">
-        <v>5.668728366339443</v>
+        <v>29.9268002042785</v>
       </c>
     </row>
     <row r="225">
@@ -3807,7 +3807,7 @@
         </is>
       </c>
       <c r="C225" t="n">
-        <v>5.610865695259445</v>
+        <v>68.38531021296235</v>
       </c>
     </row>
     <row r="226">
@@ -3822,7 +3822,7 @@
         </is>
       </c>
       <c r="C226" t="n">
-        <v>5.86589616584113</v>
+        <v>71.52815997064759</v>
       </c>
     </row>
     <row r="227">
@@ -3837,7 +3837,7 @@
         </is>
       </c>
       <c r="C227" t="n">
-        <v>6.413587679827619</v>
+        <v>63.97743836745041</v>
       </c>
     </row>
     <row r="228">
@@ -3852,7 +3852,7 @@
         </is>
       </c>
       <c r="C228" t="n">
-        <v>5.461102524471921</v>
+        <v>46.63833075734158</v>
       </c>
     </row>
     <row r="229">
@@ -3867,7 +3867,7 @@
         </is>
       </c>
       <c r="C229" t="n">
-        <v>5.600313304240797</v>
+        <v>53.61978292491888</v>
       </c>
     </row>
     <row r="230">
@@ -3882,7 +3882,7 @@
         </is>
       </c>
       <c r="C230" t="n">
-        <v>7.400050561594858</v>
+        <v>60.47527899165733</v>
       </c>
     </row>
     <row r="231">
@@ -3897,7 +3897,7 @@
         </is>
       </c>
       <c r="C231" t="n">
-        <v>6.596711669562892</v>
+        <v>58.16735730517311</v>
       </c>
     </row>
     <row r="232">
@@ -3912,7 +3912,7 @@
         </is>
       </c>
       <c r="C232" t="n">
-        <v>5.531224042890584</v>
+        <v>72.56663897908328</v>
       </c>
     </row>
     <row r="233">
@@ -3927,7 +3927,7 @@
         </is>
       </c>
       <c r="C233" t="n">
-        <v>5.585888282234356</v>
+        <v>62.47900041999161</v>
       </c>
     </row>
     <row r="234">
@@ -3942,7 +3942,7 @@
         </is>
       </c>
       <c r="C234" t="n">
-        <v>8.429451949967303</v>
+        <v>40.29955616156276</v>
       </c>
     </row>
     <row r="235">
@@ -3957,7 +3957,7 @@
         </is>
       </c>
       <c r="C235" t="n">
-        <v>6.384849261877725</v>
+        <v>54.02762005934283</v>
       </c>
     </row>
     <row r="236">
@@ -3972,7 +3972,7 @@
         </is>
       </c>
       <c r="C236" t="n">
-        <v>7.10075117054603</v>
+        <v>45.57550442954829</v>
       </c>
     </row>
     <row r="237">
@@ -3987,7 +3987,7 @@
         </is>
       </c>
       <c r="C237" t="n">
-        <v>6.651104886399003</v>
+        <v>43.71926548397136</v>
       </c>
     </row>
     <row r="238">
@@ -4002,7 +4002,7 @@
         </is>
       </c>
       <c r="C238" t="n">
-        <v>7.154314289757985</v>
+        <v>45.32952776336274</v>
       </c>
     </row>
     <row r="239">
@@ -4017,7 +4017,7 @@
         </is>
       </c>
       <c r="C239" t="n">
-        <v>6.354679802955665</v>
+        <v>37.76085982982535</v>
       </c>
     </row>
     <row r="240">
@@ -4032,7 +4032,7 @@
         </is>
       </c>
       <c r="C240" t="n">
-        <v>8.333951074870274</v>
+        <v>29.99629355077835</v>
       </c>
     </row>
     <row r="241">
@@ -4047,7 +4047,7 @@
         </is>
       </c>
       <c r="C241" t="n">
-        <v>7.423025642615732</v>
+        <v>45.37068618027348</v>
       </c>
     </row>
     <row r="242">
@@ -4062,7 +4062,7 @@
         </is>
       </c>
       <c r="C242" t="n">
-        <v>7.609785746846984</v>
+        <v>46.24525148153776</v>
       </c>
     </row>
     <row r="243">
@@ -4077,7 +4077,7 @@
         </is>
       </c>
       <c r="C243" t="n">
-        <v>7.907602053287705</v>
+        <v>39.30579320459545</v>
       </c>
     </row>
     <row r="244">
@@ -4092,7 +4092,7 @@
         </is>
       </c>
       <c r="C244" t="n">
-        <v>7.800570001055558</v>
+        <v>34.83339783962563</v>
       </c>
     </row>
     <row r="245">
@@ -4107,7 +4107,7 @@
         </is>
       </c>
       <c r="C245" t="n">
-        <v>7.215018094089263</v>
+        <v>33.73416767189385</v>
       </c>
     </row>
     <row r="246">
@@ -4122,7 +4122,7 @@
         </is>
       </c>
       <c r="C246" t="n">
-        <v>6.395425266202182</v>
+        <v>34.23820165636914</v>
       </c>
     </row>
     <row r="247">
@@ -4137,7 +4137,7 @@
         </is>
       </c>
       <c r="C247" t="n">
-        <v>7.162699362996312</v>
+        <v>36.89352938359117</v>
       </c>
     </row>
     <row r="248">
@@ -4152,7 +4152,7 @@
         </is>
       </c>
       <c r="C248" t="n">
-        <v>6.160806618407446</v>
+        <v>37.28541882109617</v>
       </c>
     </row>
     <row r="249">
@@ -4167,7 +4167,7 @@
         </is>
       </c>
       <c r="C249" t="n">
-        <v>7.016561175526055</v>
+        <v>47.82762934334099</v>
       </c>
     </row>
     <row r="250">
@@ -4182,7 +4182,7 @@
         </is>
       </c>
       <c r="C250" t="n">
-        <v>7.959559966023742</v>
+        <v>40.72593175744267</v>
       </c>
     </row>
     <row r="251">
@@ -4197,7 +4197,7 @@
         </is>
       </c>
       <c r="C251" t="n">
-        <v>8.328592104606477</v>
+        <v>36.62624145331137</v>
       </c>
     </row>
     <row r="252">
@@ -4212,7 +4212,7 @@
         </is>
       </c>
       <c r="C252" t="n">
-        <v>5.772652388797364</v>
+        <v>39.51894563426689</v>
       </c>
     </row>
     <row r="253">
@@ -4227,7 +4227,7 @@
         </is>
       </c>
       <c r="C253" t="n">
-        <v>7.066857962697275</v>
+        <v>26.68617886178862</v>
       </c>
     </row>
     <row r="254">
@@ -4242,7 +4242,7 @@
         </is>
       </c>
       <c r="C254" t="n">
-        <v>7.384606277655277</v>
+        <v>25.84834179331982</v>
       </c>
     </row>
     <row r="255">
@@ -4257,7 +4257,7 @@
         </is>
       </c>
       <c r="C255" t="n">
-        <v>6.075086939036218</v>
+        <v>33.23555156017128</v>
       </c>
     </row>
     <row r="256">
@@ -4272,7 +4272,7 @@
         </is>
       </c>
       <c r="C256" t="n">
-        <v>5.603741882748285</v>
+        <v>25.08060487716271</v>
       </c>
     </row>
     <row r="257">
@@ -4287,7 +4287,7 @@
         </is>
       </c>
       <c r="C257" t="n">
-        <v>6.793029737262223</v>
+        <v>34.0138539383608</v>
       </c>
     </row>
     <row r="258">
@@ -4302,7 +4302,7 @@
         </is>
       </c>
       <c r="C258" t="n">
-        <v>7.96187006966045</v>
+        <v>45.69441651981597</v>
       </c>
     </row>
     <row r="259">
@@ -4317,7 +4317,7 @@
         </is>
       </c>
       <c r="C259" t="n">
-        <v>7.720457082359982</v>
+        <v>41.48379152809584</v>
       </c>
     </row>
     <row r="260">
@@ -4332,7 +4332,7 @@
         </is>
       </c>
       <c r="C260" t="n">
-        <v>5.903544272749571</v>
+        <v>49.59682364483689</v>
       </c>
     </row>
     <row r="261">
@@ -4347,7 +4347,7 @@
         </is>
       </c>
       <c r="C261" t="n">
-        <v>8.206924898710144</v>
+        <v>43.18373098980251</v>
       </c>
     </row>
     <row r="262">
@@ -4362,7 +4362,7 @@
         </is>
       </c>
       <c r="C262" t="n">
-        <v>6.000702423360594</v>
+        <v>47.3031960262907</v>
       </c>
     </row>
     <row r="263">
@@ -4377,7 +4377,7 @@
         </is>
       </c>
       <c r="C263" t="n">
-        <v>6.225086168140267</v>
+        <v>49.31515060692342</v>
       </c>
     </row>
     <row r="264">
@@ -4392,7 +4392,7 @@
         </is>
       </c>
       <c r="C264" t="n">
-        <v>7.851442602823819</v>
+        <v>42.33476570493145</v>
       </c>
     </row>
     <row r="265">
@@ -4407,7 +4407,7 @@
         </is>
       </c>
       <c r="C265" t="n">
-        <v>6.431787757088962</v>
+        <v>48.74954362906171</v>
       </c>
     </row>
     <row r="266">
@@ -4422,7 +4422,7 @@
         </is>
       </c>
       <c r="C266" t="n">
-        <v>7.488005793428081</v>
+        <v>53.21082646872453</v>
       </c>
     </row>
     <row r="267">
@@ -4437,7 +4437,7 @@
         </is>
       </c>
       <c r="C267" t="n">
-        <v>6.298564546972961</v>
+        <v>45.80378107525841</v>
       </c>
     </row>
     <row r="268">
@@ -4452,7 +4452,7 @@
         </is>
       </c>
       <c r="C268" t="n">
-        <v>6.91609977324263</v>
+        <v>53.41795254687241</v>
       </c>
     </row>
     <row r="269">
@@ -4467,7 +4467,7 @@
         </is>
       </c>
       <c r="C269" t="n">
-        <v>6.444806895210163</v>
+        <v>41.92192012449685</v>
       </c>
     </row>
     <row r="270">
@@ -4482,7 +4482,7 @@
         </is>
       </c>
       <c r="C270" t="n">
-        <v>7.356621301977992</v>
+        <v>56.89554694731068</v>
       </c>
     </row>
     <row r="271">
@@ -4497,7 +4497,7 @@
         </is>
       </c>
       <c r="C271" t="n">
-        <v>7.036291434559594</v>
+        <v>51.87110473774199</v>
       </c>
     </row>
     <row r="272">
@@ -4512,7 +4512,7 @@
         </is>
       </c>
       <c r="C272" t="n">
-        <v>7.898782278262371</v>
+        <v>46.26478970550134</v>
       </c>
     </row>
     <row r="273">
@@ -4527,7 +4527,7 @@
         </is>
       </c>
       <c r="C273" t="n">
-        <v>6.61507872534795</v>
+        <v>58.13047450158525</v>
       </c>
     </row>
     <row r="274">
@@ -4542,7 +4542,7 @@
         </is>
       </c>
       <c r="C274" t="n">
-        <v>7.260617475860348</v>
+        <v>39.35075397410731</v>
       </c>
     </row>
     <row r="275">
@@ -4557,7 +4557,7 @@
         </is>
       </c>
       <c r="C275" t="n">
-        <v>6.893221464356854</v>
+        <v>39.00223335546569</v>
       </c>
     </row>
     <row r="276">
@@ -4572,7 +4572,7 @@
         </is>
       </c>
       <c r="C276" t="n">
-        <v>7.760341169303166</v>
+        <v>33.28291422449109</v>
       </c>
     </row>
     <row r="277">
@@ -4587,7 +4587,7 @@
         </is>
       </c>
       <c r="C277" t="n">
-        <v>6.046470536266455</v>
+        <v>37.37432635391819</v>
       </c>
     </row>
     <row r="278">
@@ -4602,7 +4602,7 @@
         </is>
       </c>
       <c r="C278" t="n">
-        <v>6.139982883895759</v>
+        <v>35.58807242461363</v>
       </c>
     </row>
     <row r="279">
@@ -4617,7 +4617,7 @@
         </is>
       </c>
       <c r="C279" t="n">
-        <v>7.514997355063084</v>
+        <v>31.70210131796643</v>
       </c>
     </row>
     <row r="280">
@@ -4632,7 +4632,7 @@
         </is>
       </c>
       <c r="C280" t="n">
-        <v>7.202269806241968</v>
+        <v>53.33317166622208</v>
       </c>
     </row>
     <row r="281">
@@ -4647,7 +4647,7 @@
         </is>
       </c>
       <c r="C281" t="n">
-        <v>7.056358780734874</v>
+        <v>40.72198176627682</v>
       </c>
     </row>
     <row r="282">
@@ -4662,7 +4662,7 @@
         </is>
       </c>
       <c r="C282" t="n">
-        <v>7.262255014382974</v>
+        <v>33.83242361297679</v>
       </c>
     </row>
     <row r="283">
@@ -4677,7 +4677,7 @@
         </is>
       </c>
       <c r="C283" t="n">
-        <v>6.779469825155104</v>
+        <v>43.38973491257755</v>
       </c>
     </row>
     <row r="284">
@@ -4692,7 +4692,7 @@
         </is>
       </c>
       <c r="C284" t="n">
-        <v>5.529329825104473</v>
+        <v>43.99473765670949</v>
       </c>
     </row>
     <row r="285">
@@ -4707,7 +4707,7 @@
         </is>
       </c>
       <c r="C285" t="n">
-        <v>7.605701473414478</v>
+        <v>44.2568866111467</v>
       </c>
     </row>
     <row r="286">
@@ -4722,7 +4722,7 @@
         </is>
       </c>
       <c r="C286" t="n">
-        <v>7.285820020970826</v>
+        <v>45.52519583050638</v>
       </c>
     </row>
     <row r="287">
@@ -4737,7 +4737,7 @@
         </is>
       </c>
       <c r="C287" t="n">
-        <v>7.576761652308372</v>
+        <v>35.44447600113604</v>
       </c>
     </row>
     <row r="288">
@@ -4752,7 +4752,7 @@
         </is>
       </c>
       <c r="C288" t="n">
-        <v>5.300567633930791</v>
+        <v>33.53215432485362</v>
       </c>
     </row>
     <row r="289">
@@ -4767,7 +4767,7 @@
         </is>
       </c>
       <c r="C289" t="n">
-        <v>7.599482832926303</v>
+        <v>40.01819661925968</v>
       </c>
     </row>
     <row r="290">
@@ -4782,7 +4782,7 @@
         </is>
       </c>
       <c r="C290" t="n">
-        <v>7.700128257265305</v>
+        <v>40.63409140676323</v>
       </c>
     </row>
     <row r="291">
@@ -4797,7 +4797,7 @@
         </is>
       </c>
       <c r="C291" t="n">
-        <v>9.420204111817778</v>
+        <v>36.21801508652566</v>
       </c>
     </row>
     <row r="292">
@@ -4812,7 +4812,7 @@
         </is>
       </c>
       <c r="C292" t="n">
-        <v>7.621191135734072</v>
+        <v>45.34626038781163</v>
       </c>
     </row>
     <row r="293">
@@ -4827,7 +4827,7 @@
         </is>
       </c>
       <c r="C293" t="n">
-        <v>4.666226833803155</v>
+        <v>59.49439213099023</v>
       </c>
     </row>
     <row r="294">
@@ -4842,7 +4842,7 @@
         </is>
       </c>
       <c r="C294" t="n">
-        <v>4.934117586623174</v>
+        <v>63.34215190198547</v>
       </c>
     </row>
     <row r="295">
@@ -4857,7 +4857,7 @@
         </is>
       </c>
       <c r="C295" t="n">
-        <v>4.896561988391129</v>
+        <v>59.06384878702188</v>
       </c>
     </row>
     <row r="296">
@@ -4872,7 +4872,7 @@
         </is>
       </c>
       <c r="C296" t="n">
-        <v>6.875540409948629</v>
+        <v>61.70388077920757</v>
       </c>
     </row>
     <row r="297">
@@ -4887,7 +4887,7 @@
         </is>
       </c>
       <c r="C297" t="n">
-        <v>5.147442768021547</v>
+        <v>60.56283837634319</v>
       </c>
     </row>
     <row r="298">
@@ -4902,7 +4902,7 @@
         </is>
       </c>
       <c r="C298" t="n">
-        <v>4.491275776116021</v>
+        <v>64.40516655336506</v>
       </c>
     </row>
     <row r="299">
@@ -4917,7 +4917,7 @@
         </is>
       </c>
       <c r="C299" t="n">
-        <v>5.999786939384255</v>
+        <v>49.48545861297539</v>
       </c>
     </row>
     <row r="300">
@@ -4932,7 +4932,7 @@
         </is>
       </c>
       <c r="C300" t="n">
-        <v>5.028512182477968</v>
+        <v>60.14054489948736</v>
       </c>
     </row>
     <row r="301">
@@ -4947,7 +4947,7 @@
         </is>
       </c>
       <c r="C301" t="n">
-        <v>5.944817300521999</v>
+        <v>53.66442953020134</v>
       </c>
     </row>
     <row r="302">
@@ -4962,7 +4962,7 @@
         </is>
       </c>
       <c r="C302" t="n">
-        <v>6.092000461733811</v>
+        <v>48.23098233868175</v>
       </c>
     </row>
     <row r="303">
@@ -4977,7 +4977,7 @@
         </is>
       </c>
       <c r="C303" t="n">
-        <v>6.89962216927779</v>
+        <v>53.7795105046567</v>
       </c>
     </row>
     <row r="304">
@@ -4992,7 +4992,7 @@
         </is>
       </c>
       <c r="C304" t="n">
-        <v>5.279299014238773</v>
+        <v>65.25426380848067</v>
       </c>
     </row>
     <row r="305">
@@ -5007,7 +5007,7 @@
         </is>
       </c>
       <c r="C305" t="n">
-        <v>5.414343758858546</v>
+        <v>63.73901540205991</v>
       </c>
     </row>
     <row r="306">
@@ -5022,7 +5022,7 @@
         </is>
       </c>
       <c r="C306" t="n">
-        <v>6.626109504338287</v>
+        <v>39.94315348558891</v>
       </c>
     </row>
     <row r="307">
@@ -5037,7 +5037,7 @@
         </is>
       </c>
       <c r="C307" t="n">
-        <v>4.937655860349127</v>
+        <v>41.53706642484698</v>
       </c>
     </row>
     <row r="308">
@@ -5052,7 +5052,7 @@
         </is>
       </c>
       <c r="C308" t="n">
-        <v>5.492544921626099</v>
+        <v>38.03364343061043</v>
       </c>
     </row>
     <row r="309">
@@ -5067,7 +5067,7 @@
         </is>
       </c>
       <c r="C309" t="n">
-        <v>5.374041045212041</v>
+        <v>48.21838856653297</v>
       </c>
     </row>
     <row r="310">
@@ -5082,7 +5082,7 @@
         </is>
       </c>
       <c r="C310" t="n">
-        <v>5.608011444921316</v>
+        <v>41.55937052932761</v>
       </c>
     </row>
     <row r="311">
@@ -5097,7 +5097,7 @@
         </is>
       </c>
       <c r="C311" t="n">
-        <v>8.930942895086321</v>
+        <v>43.34178437764095</v>
       </c>
     </row>
     <row r="312">
@@ -5112,7 +5112,7 @@
         </is>
       </c>
       <c r="C312" t="n">
-        <v>6.859112451529513</v>
+        <v>37.01421800947868</v>
       </c>
     </row>
     <row r="313">
@@ -5127,7 +5127,7 @@
         </is>
       </c>
       <c r="C313" t="n">
-        <v>6.679540765038887</v>
+        <v>43.91037511242791</v>
       </c>
     </row>
     <row r="314">
@@ -5142,7 +5142,7 @@
         </is>
       </c>
       <c r="C314" t="n">
-        <v>6.297452336763961</v>
+        <v>39.47190821663574</v>
       </c>
     </row>
     <row r="315">
@@ -5157,7 +5157,7 @@
         </is>
       </c>
       <c r="C315" t="n">
-        <v>6.02372420610404</v>
+        <v>39.12640553564809</v>
       </c>
     </row>
     <row r="316">
@@ -5172,7 +5172,7 @@
         </is>
       </c>
       <c r="C316" t="n">
-        <v>6.480261552725321</v>
+        <v>38.55950812472552</v>
       </c>
     </row>
     <row r="317">
@@ -5187,7 +5187,7 @@
         </is>
       </c>
       <c r="C317" t="n">
-        <v>6.264670174018616</v>
+        <v>51.74423310400648</v>
       </c>
     </row>
     <row r="318">
@@ -5202,7 +5202,7 @@
         </is>
       </c>
       <c r="C318" t="n">
-        <v>4.215443493921657</v>
+        <v>49.08262044124269</v>
       </c>
     </row>
     <row r="319">
@@ -5217,7 +5217,7 @@
         </is>
       </c>
       <c r="C319" t="n">
-        <v>6.527286196394765</v>
+        <v>47.27961149065767</v>
       </c>
     </row>
     <row r="320">
@@ -5232,7 +5232,7 @@
         </is>
       </c>
       <c r="C320" t="n">
-        <v>7.614493637125658</v>
+        <v>35.0053341461556</v>
       </c>
     </row>
     <row r="321">
@@ -5247,7 +5247,7 @@
         </is>
       </c>
       <c r="C321" t="n">
-        <v>6.094636915247603</v>
+        <v>37.63701311411235</v>
       </c>
     </row>
     <row r="322">
@@ -5262,7 +5262,7 @@
         </is>
       </c>
       <c r="C322" t="n">
-        <v>6.378581493658995</v>
+        <v>51.96806012212306</v>
       </c>
     </row>
     <row r="323">
@@ -5277,7 +5277,7 @@
         </is>
       </c>
       <c r="C323" t="n">
-        <v>6.446523968305189</v>
+        <v>45.33003477824388</v>
       </c>
     </row>
     <row r="324">
@@ -5292,7 +5292,7 @@
         </is>
       </c>
       <c r="C324" t="n">
-        <v>5.099296648738106</v>
+        <v>40.73231278444352</v>
       </c>
     </row>
     <row r="325">
@@ -5307,7 +5307,7 @@
         </is>
       </c>
       <c r="C325" t="n">
-        <v>5.685808132291313</v>
+        <v>39.58545701664968</v>
       </c>
     </row>
     <row r="326">
@@ -5322,7 +5322,7 @@
         </is>
       </c>
       <c r="C326" t="n">
-        <v>5.465395125759858</v>
+        <v>35.72026100050192</v>
       </c>
     </row>
     <row r="327">
@@ -5337,7 +5337,7 @@
         </is>
       </c>
       <c r="C327" t="n">
-        <v>6.993419454820915</v>
+        <v>31.10666497045115</v>
       </c>
     </row>
     <row r="328">
@@ -5352,7 +5352,7 @@
         </is>
       </c>
       <c r="C328" t="n">
-        <v>6.981114778144482</v>
+        <v>31.20187018701871</v>
       </c>
     </row>
     <row r="329">
@@ -5367,7 +5367,7 @@
         </is>
       </c>
       <c r="C329" t="n">
-        <v>6.231784219172274</v>
+        <v>37.88087541730698</v>
       </c>
     </row>
     <row r="330">
@@ -5382,7 +5382,7 @@
         </is>
       </c>
       <c r="C330" t="n">
-        <v>6.407005543106499</v>
+        <v>38.2356409954004</v>
       </c>
     </row>
     <row r="331">
@@ -5397,7 +5397,7 @@
         </is>
       </c>
       <c r="C331" t="n">
-        <v>9.955368212248947</v>
+        <v>45.1555913711877</v>
       </c>
     </row>
     <row r="332">
@@ -5412,7 +5412,7 @@
         </is>
       </c>
       <c r="C332" t="n">
-        <v>7.306926311130781</v>
+        <v>41.2038061518035</v>
       </c>
     </row>
     <row r="333">
@@ -5427,7 +5427,7 @@
         </is>
       </c>
       <c r="C333" t="n">
-        <v>5.575753776719113</v>
+        <v>47.91888672976869</v>
       </c>
     </row>
     <row r="334">
@@ -5442,7 +5442,7 @@
         </is>
       </c>
       <c r="C334" t="n">
-        <v>5.616408934707904</v>
+        <v>55.2539733676976</v>
       </c>
     </row>
     <row r="335">
@@ -5457,7 +5457,7 @@
         </is>
       </c>
       <c r="C335" t="n">
-        <v>5.500604047115675</v>
+        <v>43.26109936575052</v>
       </c>
     </row>
     <row r="336">
@@ -5472,7 +5472,7 @@
         </is>
       </c>
       <c r="C336" t="n">
-        <v>5.768112878507637</v>
+        <v>58.17259419753739</v>
       </c>
     </row>
     <row r="337">
@@ -5487,7 +5487,7 @@
         </is>
       </c>
       <c r="C337" t="n">
-        <v>5.404101757896241</v>
+        <v>59.12355295126483</v>
       </c>
     </row>
     <row r="338">
@@ -5502,7 +5502,7 @@
         </is>
       </c>
       <c r="C338" t="n">
-        <v>6.299474121228895</v>
+        <v>38.62994741212289</v>
       </c>
     </row>
     <row r="339">
@@ -5517,7 +5517,7 @@
         </is>
       </c>
       <c r="C339" t="n">
-        <v>6.402935171760807</v>
+        <v>44.94481758735983</v>
       </c>
     </row>
     <row r="340">
@@ -5532,7 +5532,7 @@
         </is>
       </c>
       <c r="C340" t="n">
-        <v>7.364859548351562</v>
+        <v>40.81753088362577</v>
       </c>
     </row>
     <row r="341">
@@ -5547,7 +5547,7 @@
         </is>
       </c>
       <c r="C341" t="n">
-        <v>5.931620726295393</v>
+        <v>32.48953059566223</v>
       </c>
     </row>
     <row r="342">
@@ -5562,7 +5562,7 @@
         </is>
       </c>
       <c r="C342" t="n">
-        <v>6.644623346751007</v>
+        <v>33.81253594019552</v>
       </c>
     </row>
     <row r="343">
@@ -5577,7 +5577,7 @@
         </is>
       </c>
       <c r="C343" t="n">
-        <v>6.505386505386506</v>
+        <v>32.98431298431299</v>
       </c>
     </row>
     <row r="344">
@@ -5592,7 +5592,7 @@
         </is>
       </c>
       <c r="C344" t="n">
-        <v>6.645262744070239</v>
+        <v>43.23417638579479</v>
       </c>
     </row>
     <row r="345">
@@ -5607,7 +5607,7 @@
         </is>
       </c>
       <c r="C345" t="n">
-        <v>6.182504315709181</v>
+        <v>44.44578264884179</v>
       </c>
     </row>
     <row r="346">
@@ -5622,7 +5622,7 @@
         </is>
       </c>
       <c r="C346" t="n">
-        <v>6.663768675940237</v>
+        <v>36.26352395672334</v>
       </c>
     </row>
     <row r="347">
@@ -5637,7 +5637,7 @@
         </is>
       </c>
       <c r="C347" t="n">
-        <v>5.566081578665141</v>
+        <v>46.69502734779966</v>
       </c>
     </row>
     <row r="348">
@@ -5652,7 +5652,7 @@
         </is>
       </c>
       <c r="C348" t="n">
-        <v>6.642963893727809</v>
+        <v>27.08684353314105</v>
       </c>
     </row>
     <row r="349">
@@ -5667,7 +5667,7 @@
         </is>
       </c>
       <c r="C349" t="n">
-        <v>6.319109173026008</v>
+        <v>40.71406323002648</v>
       </c>
     </row>
     <row r="350">
@@ -5682,7 +5682,7 @@
         </is>
       </c>
       <c r="C350" t="n">
-        <v>5.933440934593805</v>
+        <v>50.23825993390209</v>
       </c>
     </row>
     <row r="351">
@@ -5697,7 +5697,7 @@
         </is>
       </c>
       <c r="C351" t="n">
-        <v>6.040612687384888</v>
+        <v>33.14060569323666</v>
       </c>
     </row>
     <row r="352">
@@ -5712,7 +5712,7 @@
         </is>
       </c>
       <c r="C352" t="n">
-        <v>14.19835445852791</v>
+        <v>38.0179378845156</v>
       </c>
     </row>
     <row r="353">
@@ -5727,7 +5727,7 @@
         </is>
       </c>
       <c r="C353" t="n">
-        <v>8.299492385786802</v>
+        <v>38.5605511240029</v>
       </c>
     </row>
     <row r="354">
@@ -5742,7 +5742,7 @@
         </is>
       </c>
       <c r="C354" t="n">
-        <v>5.481640563616363</v>
+        <v>56.64973023937981</v>
       </c>
     </row>
     <row r="355">
@@ -5757,7 +5757,7 @@
         </is>
       </c>
       <c r="C355" t="n">
-        <v>7.186932849364791</v>
+        <v>36.65731727437716</v>
       </c>
     </row>
     <row r="356">
@@ -5772,7 +5772,7 @@
         </is>
       </c>
       <c r="C356" t="n">
-        <v>6.984563655815375</v>
+        <v>37.31468745223903</v>
       </c>
     </row>
     <row r="357">
@@ -5787,7 +5787,7 @@
         </is>
       </c>
       <c r="C357" t="n">
-        <v>6.975264235515468</v>
+        <v>41.28437828565104</v>
       </c>
     </row>
     <row r="358">
@@ -5802,7 +5802,7 @@
         </is>
       </c>
       <c r="C358" t="n">
-        <v>6.67092470371159</v>
+        <v>37.89652969980839</v>
       </c>
     </row>
     <row r="359">
@@ -5817,7 +5817,7 @@
         </is>
       </c>
       <c r="C359" t="n">
-        <v>6.464107246784002</v>
+        <v>34.68060767825965</v>
       </c>
     </row>
     <row r="360">
@@ -5832,7 +5832,7 @@
         </is>
       </c>
       <c r="C360" t="n">
-        <v>5.422297760355272</v>
+        <v>42.21881082266509</v>
       </c>
     </row>
     <row r="361">
@@ -5847,7 +5847,7 @@
         </is>
       </c>
       <c r="C361" t="n">
-        <v>7.414412104115913</v>
+        <v>28.11257853570971</v>
       </c>
     </row>
     <row r="362">
@@ -5862,7 +5862,7 @@
         </is>
       </c>
       <c r="C362" t="n">
-        <v>6.591771372259177</v>
+        <v>24.11398538227807</v>
       </c>
     </row>
     <row r="363">
@@ -5877,7 +5877,7 @@
         </is>
       </c>
       <c r="C363" t="n">
-        <v>5.053412298666076</v>
+        <v>37.11186140477113</v>
       </c>
     </row>
     <row r="364">
@@ -5892,7 +5892,7 @@
         </is>
       </c>
       <c r="C364" t="n">
-        <v>5.572790343504992</v>
+        <v>40.94421569180439</v>
       </c>
     </row>
     <row r="365">
@@ -5907,7 +5907,7 @@
         </is>
       </c>
       <c r="C365" t="n">
-        <v>6.006798461400841</v>
+        <v>38.38447088290545</v>
       </c>
     </row>
     <row r="366">
@@ -5922,7 +5922,7 @@
         </is>
       </c>
       <c r="C366" t="n">
-        <v>6.436191919780796</v>
+        <v>36.60584154375328</v>
       </c>
     </row>
     <row r="367">
@@ -5937,7 +5937,7 @@
         </is>
       </c>
       <c r="C367" t="n">
-        <v>5.495694138203603</v>
+        <v>37.61284686108915</v>
       </c>
     </row>
     <row r="368">
@@ -5952,7 +5952,7 @@
         </is>
       </c>
       <c r="C368" t="n">
-        <v>6.46336193592197</v>
+        <v>42.53966294215692</v>
       </c>
     </row>
     <row r="369">
@@ -5967,7 +5967,7 @@
         </is>
       </c>
       <c r="C369" t="n">
-        <v>5.108582219350991</v>
+        <v>36.17750832380857</v>
       </c>
     </row>
     <row r="370">
@@ -5982,7 +5982,7 @@
         </is>
       </c>
       <c r="C370" t="n">
-        <v>5.406373992064508</v>
+        <v>36.34199411237681</v>
       </c>
     </row>
     <row r="371">
@@ -5997,7 +5997,7 @@
         </is>
       </c>
       <c r="C371" t="n">
-        <v>7.082474959153229</v>
+        <v>37.17766569581587</v>
       </c>
     </row>
     <row r="372">
@@ -6012,7 +6012,7 @@
         </is>
       </c>
       <c r="C372" t="n">
-        <v>6.722459035626295</v>
+        <v>38.43807438113488</v>
       </c>
     </row>
     <row r="373">
@@ -6027,7 +6027,7 @@
         </is>
       </c>
       <c r="C373" t="n">
-        <v>7.332554310299039</v>
+        <v>29.90120571519626</v>
       </c>
     </row>
     <row r="374">
@@ -6042,7 +6042,7 @@
         </is>
       </c>
       <c r="C374" t="n">
-        <v>5.69263648727414</v>
+        <v>48.46188718347258</v>
       </c>
     </row>
     <row r="375">
@@ -6057,7 +6057,7 @@
         </is>
       </c>
       <c r="C375" t="n">
-        <v>5.84732231476287</v>
+        <v>39.80494541060717</v>
       </c>
     </row>
     <row r="376">
@@ -6072,7 +6072,7 @@
         </is>
       </c>
       <c r="C376" t="n">
-        <v>7.048790392759761</v>
+        <v>37.84494594960453</v>
       </c>
     </row>
     <row r="377">
@@ -6087,7 +6087,7 @@
         </is>
       </c>
       <c r="C377" t="n">
-        <v>6.79460074808912</v>
+        <v>41.49292567897219</v>
       </c>
     </row>
     <row r="378">
@@ -6102,7 +6102,7 @@
         </is>
       </c>
       <c r="C378" t="n">
-        <v>5.449950554884079</v>
+        <v>41.58334248983628</v>
       </c>
     </row>
     <row r="379">
@@ -6117,7 +6117,7 @@
         </is>
       </c>
       <c r="C379" t="n">
-        <v>6.200119942796512</v>
+        <v>35.85828297273608</v>
       </c>
     </row>
     <row r="380">
@@ -6132,7 +6132,7 @@
         </is>
       </c>
       <c r="C380" t="n">
-        <v>5.31132783195799</v>
+        <v>40.57014253563391</v>
       </c>
     </row>
     <row r="381">
@@ -6147,7 +6147,7 @@
         </is>
       </c>
       <c r="C381" t="n">
-        <v>5.9553491558973</v>
+        <v>29.58641822576654</v>
       </c>
     </row>
     <row r="382">
@@ -6162,7 +6162,7 @@
         </is>
       </c>
       <c r="C382" t="n">
-        <v>6.7944233103181</v>
+        <v>32.125118560749</v>
       </c>
     </row>
     <row r="383">
@@ -6177,7 +6177,7 @@
         </is>
       </c>
       <c r="C383" t="n">
-        <v>5.323327961321515</v>
+        <v>30.17727639000806</v>
       </c>
     </row>
   </sheetData>

</xml_diff>